<commit_message>
Project Tutorial 8 - Introduction to Smart Rules and Smart Lookup Tables is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/ddd/qwdqw/qdwqwq/Tutorial 8 - Introduction to Smart Rules and Smart Lookup Tables/Tutorial8 - Introduction to Smart Rules and Smart Lookup Tables.xlsx
+++ b/ddd/qwdqw/qdwqwq/Tutorial 8 - Introduction to Smart Rules and Smart Lookup Tables/Tutorial8 - Introduction to Smart Rules and Smart Lookup Tables.xlsx
@@ -1772,7 +1772,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.499984740745262" rgb="FFFFFF"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1892,7 +1892,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -1936,7 +1936,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -9460,8 +9460,8 @@
       <c r="D59" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="E59" s="7">
-        <v>1.6</v>
+      <c r="E59" s="7" t="n">
+        <v>1.64</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>

</xml_diff>